<commit_message>
add the prediction metrics for the LSTM models
</commit_message>
<xml_diff>
--- a/Experiments Overview.xlsx
+++ b/Experiments Overview.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="138">
   <si>
     <t xml:space="preserve">Experiment Overview</t>
   </si>
@@ -132,6 +132,11 @@
     <t xml:space="preserve">Val Acc: 83.34</t>
   </si>
   <si>
+    <t xml:space="preserve">Precision: 79%
+Recall: 84%
+F1: 78%</t>
+  </si>
+  <si>
     <t xml:space="preserve">SMOTE</t>
   </si>
   <si>
@@ -150,9 +155,6 @@
 F1: 94%</t>
   </si>
   <si>
-    <t xml:space="preserve">Val Acc: 93%</t>
-  </si>
-  <si>
     <t xml:space="preserve">V1</t>
   </si>
   <si>
@@ -176,7 +178,9 @@
 F1: 83%</t>
   </si>
   <si>
-    <t xml:space="preserve">Val Acc: 85.5%</t>
+    <t xml:space="preserve">Precision: 86%
+Recall: 85%
+F1: 85%</t>
   </si>
   <si>
     <t xml:space="preserve">V2</t>
@@ -197,7 +201,9 @@
 F1: 75%</t>
   </si>
   <si>
-    <t xml:space="preserve">Val Acc: 78.3%</t>
+    <t xml:space="preserve">Precision: 78%
+Recall: 78%
+F1: 78%</t>
   </si>
   <si>
     <t xml:space="preserve">V3</t>
@@ -227,7 +233,9 @@
     <t xml:space="preserve">V6</t>
   </si>
   <si>
-    <t xml:space="preserve">Val Acc: 85.8%</t>
+    <t xml:space="preserve">Precision: 86%
+Recall: 85%
+F1: 86%</t>
   </si>
   <si>
     <t xml:space="preserve">V7</t>
@@ -244,6 +252,11 @@
     <t xml:space="preserve">Precision: 85%
 Recall: 84%
 F1: 84%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precision: 86%
+Recall: 86%
+F1: 86%</t>
   </si>
   <si>
     <t xml:space="preserve">V10</t>
@@ -791,9 +804,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>747720</xdr:colOff>
+      <xdr:colOff>747360</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>124920</xdr:rowOff>
+      <xdr:rowOff>124560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -807,7 +820,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="117000" y="156240"/>
-          <a:ext cx="2230920" cy="2894760"/>
+          <a:ext cx="2192400" cy="2894400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -828,9 +841,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>757440</xdr:colOff>
+      <xdr:colOff>757080</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>138960</xdr:rowOff>
+      <xdr:rowOff>138600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -843,8 +856,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3206880" y="0"/>
-          <a:ext cx="2351160" cy="3065040"/>
+          <a:off x="3130560" y="0"/>
+          <a:ext cx="2312640" cy="3064680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -865,9 +878,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>763560</xdr:colOff>
+      <xdr:colOff>763200</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>138960</xdr:rowOff>
+      <xdr:rowOff>138600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -880,8 +893,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6400800" y="0"/>
-          <a:ext cx="2363760" cy="3065040"/>
+          <a:off x="6248160" y="0"/>
+          <a:ext cx="2325240" cy="3064680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -907,9 +920,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>6480</xdr:colOff>
+      <xdr:colOff>6120</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>158040</xdr:rowOff>
+      <xdr:rowOff>157680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -923,7 +936,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2406600" cy="9098640"/>
+          <a:ext cx="2349000" cy="9098280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -944,9 +957,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>5760</xdr:colOff>
+      <xdr:colOff>5400</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>132120</xdr:rowOff>
+      <xdr:rowOff>131760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -959,8 +972,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3206520" y="0"/>
-          <a:ext cx="2399760" cy="9072720"/>
+          <a:off x="3130200" y="0"/>
+          <a:ext cx="2342520" cy="9072360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -981,9 +994,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>2880</xdr:colOff>
+      <xdr:colOff>2520</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>132120</xdr:rowOff>
+      <xdr:rowOff>131760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -996,8 +1009,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6406920" y="11880"/>
-          <a:ext cx="2396880" cy="9060840"/>
+          <a:off x="6254280" y="11880"/>
+          <a:ext cx="2339640" cy="9060480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1023,9 +1036,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>702360</xdr:colOff>
+      <xdr:colOff>702000</xdr:colOff>
       <xdr:row>95</xdr:row>
-      <xdr:rowOff>137880</xdr:rowOff>
+      <xdr:rowOff>137520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1039,7 +1052,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2302560" cy="15580800"/>
+          <a:ext cx="2264040" cy="15580440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1060,9 +1073,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>701280</xdr:colOff>
+      <xdr:colOff>700920</xdr:colOff>
       <xdr:row>95</xdr:row>
-      <xdr:rowOff>132120</xdr:rowOff>
+      <xdr:rowOff>131760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1075,8 +1088,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3200400" y="0"/>
-          <a:ext cx="2301480" cy="15575040"/>
+          <a:off x="3124080" y="0"/>
+          <a:ext cx="2262960" cy="15574680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1097,9 +1110,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>700560</xdr:colOff>
+      <xdr:colOff>700200</xdr:colOff>
       <xdr:row>95</xdr:row>
-      <xdr:rowOff>126000</xdr:rowOff>
+      <xdr:rowOff>125640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1112,8 +1125,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6400800" y="0"/>
-          <a:ext cx="2300760" cy="15568920"/>
+          <a:off x="6248160" y="0"/>
+          <a:ext cx="2262240" cy="15568560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1139,9 +1152,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>756000</xdr:colOff>
+      <xdr:colOff>755640</xdr:colOff>
       <xdr:row>377</xdr:row>
-      <xdr:rowOff>96480</xdr:rowOff>
+      <xdr:rowOff>96120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1155,7 +1168,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="3956400" cy="61381440"/>
+          <a:ext cx="3879720" cy="61381080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1176,9 +1189,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>585000</xdr:colOff>
+      <xdr:colOff>584640</xdr:colOff>
       <xdr:row>377</xdr:row>
-      <xdr:rowOff>30240</xdr:rowOff>
+      <xdr:rowOff>29880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1191,8 +1204,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4805640" y="0"/>
-          <a:ext cx="3780360" cy="61315200"/>
+          <a:off x="4691160" y="0"/>
+          <a:ext cx="3703680" cy="61314840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1213,9 +1226,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>736920</xdr:colOff>
+      <xdr:colOff>736560</xdr:colOff>
       <xdr:row>377</xdr:row>
-      <xdr:rowOff>113400</xdr:rowOff>
+      <xdr:rowOff>113040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1228,8 +1241,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9601200" y="0"/>
-          <a:ext cx="3937320" cy="61398360"/>
+          <a:off x="9372600" y="0"/>
+          <a:ext cx="3860640" cy="61398000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1255,9 +1268,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>326880</xdr:colOff>
+      <xdr:colOff>326520</xdr:colOff>
       <xdr:row>1480</xdr:row>
-      <xdr:rowOff>85680</xdr:rowOff>
+      <xdr:rowOff>85320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1271,7 +1284,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="5203440" cy="240674400"/>
+          <a:ext cx="5127120" cy="240674040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1297,9 +1310,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>386280</xdr:colOff>
+      <xdr:colOff>385920</xdr:colOff>
       <xdr:row>1927</xdr:row>
-      <xdr:rowOff>75600</xdr:rowOff>
+      <xdr:rowOff>75240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1313,7 +1326,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="4386600" cy="313328520"/>
+          <a:ext cx="4290840" cy="313328160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1335,14 +1348,15 @@
   </sheetPr>
   <dimension ref="A1:U18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q19" activeCellId="0" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="21" min="2" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="21" min="2" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1493,7 +1507,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="13" t="s">
         <v>28</v>
       </c>
@@ -1528,20 +1542,22 @@
       </c>
       <c r="O5" s="14"/>
       <c r="P5" s="14"/>
-      <c r="Q5" s="14"/>
+      <c r="Q5" s="17" t="s">
+        <v>32</v>
+      </c>
       <c r="R5" s="14"/>
       <c r="S5" s="14"/>
       <c r="T5" s="14"/>
       <c r="U5" s="14"/>
     </row>
-    <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="13"/>
       <c r="B6" s="14"/>
       <c r="C6" s="14" t="s">
         <v>29</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E6" s="15" t="n">
         <v>1024</v>
@@ -1559,27 +1575,27 @@
       <c r="J6" s="15"/>
       <c r="K6" s="14"/>
       <c r="L6" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="M6" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N6" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="O6" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="17" t="s">
         <v>35</v>
-      </c>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="14" t="s">
-        <v>36</v>
       </c>
       <c r="R6" s="14"/>
       <c r="S6" s="14"/>
       <c r="T6" s="14"/>
       <c r="U6" s="14"/>
     </row>
-    <row r="7" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="13" t="s">
         <v>37</v>
       </c>
@@ -1618,7 +1634,7 @@
         <v>39</v>
       </c>
       <c r="P7" s="14"/>
-      <c r="Q7" s="14" t="s">
+      <c r="Q7" s="17" t="s">
         <v>42</v>
       </c>
       <c r="R7" s="14"/>
@@ -1626,7 +1642,7 @@
       <c r="T7" s="14"/>
       <c r="U7" s="14"/>
     </row>
-    <row r="8" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="s">
         <v>43</v>
       </c>
@@ -1665,7 +1681,7 @@
         <v>45</v>
       </c>
       <c r="P8" s="14"/>
-      <c r="Q8" s="14" t="s">
+      <c r="Q8" s="17" t="s">
         <v>47</v>
       </c>
       <c r="R8" s="14"/>
@@ -1673,7 +1689,7 @@
       <c r="T8" s="14"/>
       <c r="U8" s="14"/>
     </row>
-    <row r="9" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="s">
         <v>48</v>
       </c>
@@ -1706,7 +1722,7 @@
       <c r="T9" s="14"/>
       <c r="U9" s="14"/>
     </row>
-    <row r="10" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="s">
         <v>50</v>
       </c>
@@ -1739,7 +1755,7 @@
       <c r="T10" s="14"/>
       <c r="U10" s="14"/>
     </row>
-    <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="13" t="s">
         <v>51</v>
       </c>
@@ -1778,15 +1794,15 @@
         <v>39</v>
       </c>
       <c r="P11" s="14"/>
-      <c r="Q11" s="14" t="s">
-        <v>42</v>
+      <c r="Q11" s="17" t="s">
+        <v>53</v>
       </c>
       <c r="R11" s="14"/>
       <c r="S11" s="14"/>
       <c r="T11" s="14"/>
       <c r="U11" s="14"/>
     </row>
-    <row r="12" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="13" t="s">
         <v>54</v>
       </c>
@@ -1825,7 +1841,7 @@
         <v>39</v>
       </c>
       <c r="P12" s="14"/>
-      <c r="Q12" s="14" t="s">
+      <c r="Q12" s="17" t="s">
         <v>55</v>
       </c>
       <c r="R12" s="14"/>
@@ -1833,7 +1849,7 @@
       <c r="T12" s="14"/>
       <c r="U12" s="14"/>
     </row>
-    <row r="13" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="s">
         <v>56</v>
       </c>
@@ -1874,7 +1890,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="13" t="s">
         <v>58</v>
       </c>
@@ -1913,17 +1929,17 @@
         <v>41</v>
       </c>
       <c r="P14" s="14"/>
-      <c r="Q14" s="14" t="s">
-        <v>55</v>
+      <c r="Q14" s="17" t="s">
+        <v>60</v>
       </c>
       <c r="R14" s="14"/>
       <c r="S14" s="14"/>
       <c r="T14" s="14"/>
       <c r="U14" s="14"/>
     </row>
-    <row r="15" customFormat="false" ht="29.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="13" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B15" s="14"/>
       <c r="C15" s="17" t="s">
@@ -1938,7 +1954,7 @@
       <c r="H15" s="15"/>
       <c r="I15" s="15"/>
       <c r="J15" s="18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K15" s="14"/>
       <c r="L15" s="14"/>
@@ -1946,28 +1962,28 @@
       <c r="N15" s="14"/>
       <c r="O15" s="14"/>
       <c r="P15" s="19" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="Q15" s="19" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="R15" s="19" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="S15" s="19" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="T15" s="14"/>
       <c r="U15" s="14"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -2009,7 +2025,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2035,9 +2051,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2062,9 +2075,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2089,9 +2099,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2116,9 +2123,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2143,9 +2147,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2170,434 +2171,431 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="e">
-        <f aca="false">===============================================================</f>
+        <f aca="false">==============================================================</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="e">
-        <f aca="false">===============================================================</f>
+        <f aca="false">==============================================================</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="e">
-        <f aca="false">===============================================================</f>
+        <f aca="false">==============================================================</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="e">
-        <f aca="false">===============================================================</f>
+        <f aca="false">==============================================================</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="e">
-        <f aca="false">===============================================================</f>
+        <f aca="false">==============================================================</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="e">
-        <f aca="false">===============================================================</f>
+        <f aca="false">==============================================================</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2623,155 +2621,152 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="e">
-        <f aca="false">===============================================================</f>
+        <f aca="false">==============================================================</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="e">
-        <f aca="false">===============================================================</f>
+        <f aca="false">==============================================================</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2797,165 +2792,162 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="e">
-        <f aca="false">===============================================================</f>
+        <f aca="false">==============================================================</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="e">
-        <f aca="false">===============================================================</f>
+        <f aca="false">==============================================================</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2981,150 +2973,147 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="e">
-        <f aca="false">===============================================================</f>
+        <f aca="false">==============================================================</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="e">
-        <f aca="false">===============================================================</f>
+        <f aca="false">==============================================================</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>